<commit_message>
Added power and distribution board enclosure part
</commit_message>
<xml_diff>
--- a/Other Docs/Full Parts List.xlsx
+++ b/Other Docs/Full Parts List.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AJ992\Documents\My Projects\DAMPING_ADJUSTER\Planning Docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AJ992\Documents\My Projects\DAMPING_ADJUSTER\Other Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B045CF5-77A9-4A96-9A82-871922DC3D59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF9F3502-DF95-4F35-89EB-81F54DF67083}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1144EA35-95AE-4760-990E-F9170137133D}"/>
+    <workbookView xWindow="-26070" yWindow="2730" windowWidth="21600" windowHeight="11385" xr2:uid="{1144EA35-95AE-4760-990E-F9170137133D}"/>
   </bookViews>
   <sheets>
     <sheet name="Parts" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="105">
   <si>
     <t>Part Num</t>
   </si>
@@ -345,6 +345,15 @@
   </si>
   <si>
     <t>JTAG Socket</t>
+  </si>
+  <si>
+    <t>Power and Signal Board Case Bottom</t>
+  </si>
+  <si>
+    <t>Power and signal board case top</t>
+  </si>
+  <si>
+    <t>]</t>
   </si>
 </sst>
 </file>
@@ -759,10 +768,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72027582-7337-45D0-8AEF-3D65ED56EAD2}">
-  <dimension ref="A1:G38"/>
+  <dimension ref="A1:G41"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="A39" sqref="A39"/>
+      <selection activeCell="A41" sqref="A41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1407,6 +1416,33 @@
       </c>
       <c r="F38">
         <v>0.76</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>1031</v>
+      </c>
+      <c r="C39" t="s">
+        <v>38</v>
+      </c>
+      <c r="E39" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>1032</v>
+      </c>
+      <c r="C40" t="s">
+        <v>38</v>
+      </c>
+      <c r="E40" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>104</v>
       </c>
     </row>
   </sheetData>

</xml_diff>